<commit_message>
add Wang and Zavisic papers to meta-analysis compiled datasheet
</commit_message>
<xml_diff>
--- a/np_fert_exps_in_meta_analysis.xlsx
+++ b/np_fert_exps_in_meta_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354B5B4F-D262-3B4E-8538-C03FCFF19EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D642E618-9262-B344-AEED-6B18C1D94F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="680" windowWidth="27240" windowHeight="24780" xr2:uid="{0365B344-5F90-A544-B745-15FA7234BD65}"/>
+    <workbookView xWindow="5020" yWindow="1980" windowWidth="37780" windowHeight="26820" xr2:uid="{0365B344-5F90-A544-B745-15FA7234BD65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="99">
   <si>
     <t>authors</t>
   </si>
@@ -248,9 +248,6 @@
     <t>P addition experiment with 2 levels: 0P and a 1/3 strength Hewitt's olution (0.44 mM NaH2PO4 as P addition substrate). 0P solution also as modified Hewitt's solution, but without NaH2PO4)</t>
   </si>
   <si>
-    <t>data received from Keith Bloomfield on 1/6/24</t>
-  </si>
-  <si>
     <t>Zavišić et al.</t>
   </si>
   <si>
@@ -293,14 +290,56 @@
     <t>Nutrient Network fertilization scheme</t>
   </si>
   <si>
-    <t>fiedl</t>
+    <t>Cleland et al.</t>
+  </si>
+  <si>
+    <t>Belowground biomass response to nutrient enrichment depends on light limitation across globally distributed grasslands</t>
+  </si>
+  <si>
+    <t>Ecosystems</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10021-019-00350-4</t>
+  </si>
+  <si>
+    <t>root mass fraction, belowground biomass, aboveground biomass (estimated using rmf and bgb)</t>
+  </si>
+  <si>
+    <t>Wang et al.</t>
+  </si>
+  <si>
+    <t>Effects of nutrient addition on foliar phosphorus fractions and their resorption in different-aged leaves of Chinese fir in subtropical China</t>
+  </si>
+  <si>
+    <t>Plant and Soil</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11104-019-04221-8</t>
+  </si>
+  <si>
+    <t>n; mean and SE reported in supplemental table</t>
+  </si>
+  <si>
+    <t>leaf phosphorus fractions (Pi, sugar P, nucleic P, residual P), Nmass, Pmass</t>
+  </si>
+  <si>
+    <t>Two nitrogen addition treatments (N1 = 50 kg N/ha/yr, N2 = 100 kg N/ha/yr) and one phosphorus treatment (50 kg P/ha/yr) in full factorial setup (i.e. N1, N2, P, N1P, N2P, Control)</t>
+  </si>
+  <si>
+    <t>summary table copied from supplemental table, then cleaned in R to make for easy load into compiled data file</t>
+  </si>
+  <si>
+    <t>summary table cleaned in R to make for easy load into compiled data file</t>
+  </si>
+  <si>
+    <t>data received from Keith Bloomfield on 1/6/24; summary table cleaned in R to make for easy load into compiled data file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -356,13 +395,32 @@
       <color rgb="FF000000"/>
       <name val="Aptos"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -393,48 +451,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1051,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DA6B57-0823-4F41-93CF-4F8606F480FC}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1067,405 +1130,480 @@
     <col min="6" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="2">
         <v>2024</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="8"/>
+      <c r="J2" s="14" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>2019</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="8"/>
+      <c r="J3" s="14" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <v>2021</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="11">
         <v>2022</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="4">
         <v>2022</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="8"/>
+      <c r="J6" s="14" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="5">
         <v>2017</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="8"/>
+      <c r="I7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="5">
         <v>2007</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="8"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="2">
         <v>2002</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="8"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="2">
         <v>2011</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="8"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="4">
         <v>2014</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>70</v>
+      <c r="J11" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="9">
-        <v>2018</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="8" t="s">
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>77</v>
+      <c r="B13" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="9">
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="8">
         <v>2019</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="C14" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="H14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="14"/>
+      <c r="J14" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="221" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2019</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A13:B13 D13 F13:I13">

</xml_diff>

<commit_message>
add figs to digitize
</commit_message>
<xml_diff>
--- a/np_fert_exps_in_meta_analysis.xlsx
+++ b/np_fert_exps_in_meta_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/p_meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE706A-1A49-0049-A2C5-BA0DD5CB9B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D00C5E3-EE18-F845-ABB5-A7D2ABC182A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="500" windowWidth="48280" windowHeight="26820" xr2:uid="{0365B344-5F90-A544-B745-15FA7234BD65}"/>
+    <workbookView xWindow="1180" yWindow="760" windowWidth="24980" windowHeight="18880" xr2:uid="{0365B344-5F90-A544-B745-15FA7234BD65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="134">
   <si>
     <t>authors</t>
   </si>
@@ -375,6 +375,69 @@
   </si>
   <si>
     <t>NP full factorial design with N added at rate of 10 g/m2/yr and P added at rate of 5 g P/m2/yr</t>
+  </si>
+  <si>
+    <t>Hayes et al.</t>
+  </si>
+  <si>
+    <t>Leaf phosphorus fractionation in rice to understand internal phosphorus-use efficiency</t>
+  </si>
+  <si>
+    <t>Annals of Botany</t>
+  </si>
+  <si>
+    <t>asat, ppue, leaf p fractionation, total biomass, root:shoot</t>
+  </si>
+  <si>
+    <t>P experiment with 5 rice genotypes</t>
+  </si>
+  <si>
+    <t>n; asat mean and se reported in main text</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/aob/mcab138</t>
+  </si>
+  <si>
+    <t>Black et al.</t>
+  </si>
+  <si>
+    <t>Effect of mycorrhizal-enhanced leaf phosphate status on carbon partitioning, translocation and photosynthesis in cucumber</t>
+  </si>
+  <si>
+    <t>Plant, Cell and Environment</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1046/j.1365-3040.2000.00598.x</t>
+  </si>
+  <si>
+    <t>asat, vcmax, jmax, rd, leaf N, leaf P, root biomass, total biomass, root:shoot</t>
+  </si>
+  <si>
+    <t>Ostertag</t>
+  </si>
+  <si>
+    <t>Foliar nitrogen and phosphorus accumulation responses after fertilization: an example from nutrient-limited Hawaiian forests</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11104-010-0281-x</t>
+  </si>
+  <si>
+    <t>inorganic, organic leaf phosphorus</t>
+  </si>
+  <si>
+    <t>NP full factorial design</t>
+  </si>
+  <si>
+    <t>Harrington et al.</t>
+  </si>
+  <si>
+    <t>Production and resource use efficiencies in N- and P-limited tropical forests: a comparison of responses to long-term fertilization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1007/s10021-001-0034-z </t>
+  </si>
+  <si>
+    <t>pnue, ppue, pmass, nmass, lma</t>
   </si>
 </sst>
 </file>
@@ -465,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -489,10 +552,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -502,7 +580,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -549,15 +627,21 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1202,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DA6B57-0823-4F41-93CF-4F8606F480FC}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1661,7 +1745,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="221" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>88</v>
       </c>
@@ -1694,68 +1778,190 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="8">
         <v>2024</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="J16" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="8">
         <v>2023</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="J17" s="8" t="s">
         <v>101</v>
       </c>
+    </row>
+    <row r="18" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="19">
+        <v>2000</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G19" s="22"/>
+      <c r="H19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2010</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="17">
+        <v>2001</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A13:B13 D13 F13:I13">
@@ -1924,6 +2130,8 @@
     <hyperlink ref="E11" r:id="rId9" xr:uid="{F642F8E4-E507-3C4A-B6AF-024D7104CEAB}"/>
     <hyperlink ref="E12" r:id="rId10" xr:uid="{0FCF2EC9-6C52-AD44-BEBA-34EC3B2A1036}"/>
     <hyperlink ref="E16" r:id="rId11" xr:uid="{24E31B74-0314-054D-A689-36FE555CA996}"/>
+    <hyperlink ref="E18" r:id="rId12" xr:uid="{60421007-4FA8-8843-9602-DFD6C4455CFD}"/>
+    <hyperlink ref="E19" r:id="rId13" xr:uid="{33E082FA-2A0C-9D43-8732-26D5BD32035C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>